<commit_message>
thêm của Tuấn Anh
</commit_message>
<xml_diff>
--- a/Tuan1.xlsx
+++ b/Tuan1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="58">
   <si>
     <t>大項目</t>
   </si>
@@ -181,6 +181,15 @@
   </si>
   <si>
     <t>Lam</t>
+  </si>
+  <si>
+    <t>全部会議室の状態を表す</t>
+  </si>
+  <si>
+    <t>会議室がいつからいつまで予約られたか、予約られなかったかを表す。会議室の状態を変わることを表す。</t>
+  </si>
+  <si>
+    <t>この時間予約られない会議室を計算できる。この会議室いつ予約しますかいつ予約できませんか</t>
   </si>
 </sst>
 </file>
@@ -841,7 +850,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1459,15 +1470,34 @@
       <c r="A24" s="12" t="s">
         <v>48</v>
       </c>
+      <c r="C24" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="25" spans="1:26">
       <c r="B25" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="C25" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" ht="60">
+      <c r="C26" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="27" spans="1:26">
       <c r="B27" s="4" t="s">
         <v>27</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" ht="45">
+      <c r="C28" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:26" s="43" customFormat="1">

</xml_diff>